<commit_message>
first name, second name -> full name
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/template_1.xlsx
+++ b/src/main/resources/templates/template_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavelkozlov/IdeaProjects/brackets-excel/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EABAB2-5469-B54E-9236-E75E54A5AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CC6CD0-07C3-DE44-A3FE-A6736239A00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{15E37D56-E58C-6546-B516-633D8AAEFA79}"/>
   </bookViews>
@@ -77,13 +77,13 @@
     <t>${weightCategory}</t>
   </si>
   <si>
-    <t>${graph.get("ZERO").get(0).participant.lastName} ${graph.get("ZERO").get(0).participant.firstName} ${graph.get("ZERO").get(0).participant.team? "(" + graph.get("ZERO").get(0).participant.team + ")" : null}</t>
-  </si>
-  <si>
     <t>Вес кат.</t>
   </si>
   <si>
     <t>Возр кат.</t>
+  </si>
+  <si>
+    <t>${graph.get("ZERO").get(0).participant.fullName} ${graph.get("ZERO").get(0).participant.team? "(" + graph.get("ZERO").get(0).participant.team + ")" : null}</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,7 +592,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="1"/>
       <c r="N3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>5</v>
@@ -630,7 +630,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>6</v>
@@ -807,7 +807,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="6"/>
       <c r="H22" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>

</xml_diff>